<commit_message>
added animations and started implementation of stages
</commit_message>
<xml_diff>
--- a/Mappe.xlsx
+++ b/Mappe.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="3x3" sheetId="1" r:id="rId1"/>
     <sheet name="4x4" sheetId="2" r:id="rId2"/>
     <sheet name="5x5" sheetId="3" r:id="rId3"/>
     <sheet name="6X6" sheetId="4" r:id="rId4"/>
-    <sheet name="8X8" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -3667,7 +3666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
@@ -3990,6 +3989,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="D4:E4"/>
@@ -3997,11 +4001,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4438,11 +4437,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E5:E6"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="F11:F12"/>
@@ -4450,13 +4451,11 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4466,7 +4465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5024,17 +5023,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B11:B12"/>
@@ -5049,22 +5037,18 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B23:C23"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
finished Timer mapping; texture fixing (prevented stuttering)
</commit_message>
<xml_diff>
--- a/Mappe.xlsx
+++ b/Mappe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="3x3" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,6 +187,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3989,11 +3992,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="D4:E4"/>
@@ -4001,6 +3999,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D11:E11"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4010,7 +4013,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4104,10 +4109,10 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4436,7 +4441,19 @@
       <c r="G23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="D2:E2"/>
@@ -4444,18 +4461,7 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4465,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5023,6 +5029,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B11:B12"/>
@@ -5037,17 +5054,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>